<commit_message>
Added employee status filter in user master and all MIS Implemented employee status in all MIS Exports
</commit_message>
<xml_diff>
--- a/mainadminhtml/samplefile/MIS/annualdiscloser.xlsx
+++ b/mainadminhtml/samplefile/MIS/annualdiscloser.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\drreddys\mainadminhtml\samplefile\MIS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -34,12 +39,15 @@
   </si>
   <si>
     <t>Email ID</t>
+  </si>
+  <si>
+    <t>Employee Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,7 +357,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -357,22 +365,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="2" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -380,12 +388,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>